<commit_message>
add more features data
</commit_message>
<xml_diff>
--- a/documents/payment.xlsx
+++ b/documents/payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\AbArts\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA7E9D8-D6B9-417E-885F-380824690BD9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062C4BA3-8F0E-4B1D-A1A7-2ADFB6CDA74B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">EXPERIMENTER NAME:   </t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -112,6 +112,33 @@
   <si>
     <t>anulhda@caltech.edu</t>
   </si>
+  <si>
+    <t>William Hargis</t>
+  </si>
+  <si>
+    <t>willia.hargis@gmail.com</t>
+  </si>
+  <si>
+    <t>Abigail Crites</t>
+  </si>
+  <si>
+    <t>abbycrites@gmail.com</t>
+  </si>
+  <si>
+    <t>Frank Mocabenta</t>
+  </si>
+  <si>
+    <t>Chloe Christiansen</t>
+  </si>
+  <si>
+    <t>chloechristiansen@hotmail.com</t>
+  </si>
+  <si>
+    <t>Meagan Gourley</t>
+  </si>
+  <si>
+    <t>meagan.gousley@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +151,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="000000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -172,6 +199,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -300,7 +332,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -350,7 +382,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="28"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -716,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -839,7 +876,7 @@
       <c r="A15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -850,102 +887,143 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="20">
+        <v>41831</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="20">
+        <v>41832</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="14">
+        <v>60</v>
+      </c>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="20">
+        <v>41832</v>
+      </c>
+      <c r="C18" s="22">
+        <v>2000180</v>
+      </c>
+      <c r="D18" s="26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="20">
+        <v>41833</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="20">
+        <v>41833</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="20"/>
       <c r="C21" s="22"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="20"/>
       <c r="C22" s="22"/>
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
       <c r="C23" s="22"/>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="20"/>
       <c r="C24" s="22"/>
       <c r="D24" s="14"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="22"/>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="20"/>
       <c r="C26" s="22"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="20"/>
       <c r="C27" s="22"/>
       <c r="D27" s="18"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="20"/>
       <c r="C28" s="22"/>
       <c r="D28" s="18"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="20"/>
       <c r="C29" s="22"/>
       <c r="D29" s="18"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
       <c r="D30" s="18"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="20"/>
       <c r="C31" s="22"/>
       <c r="D31" s="18"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
@@ -1109,7 +1187,7 @@
       </c>
       <c r="D58" s="12">
         <f>SUM(D12:D57)</f>
-        <v>240</v>
+        <v>540</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -1125,9 +1203,13 @@
     <hyperlink ref="C13" r:id="rId1" xr:uid="{34CEBA42-09DA-40F5-A113-24AC36B19CBE}"/>
     <hyperlink ref="C14" r:id="rId2" display="mailto:ytumaykina@aol.com" xr:uid="{17C8C095-970F-48B4-9AB0-F246238D3C05}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{1F458DBE-9E49-4ACC-BE64-98E0AF3C8BDA}"/>
+    <hyperlink ref="C16" r:id="rId4" xr:uid="{51ED8613-A9AE-4E5B-BD06-50A925868ECC}"/>
+    <hyperlink ref="C17" r:id="rId5" xr:uid="{479AE753-7857-4CC7-8CDF-D144E4FD53C7}"/>
+    <hyperlink ref="C19" r:id="rId6" xr:uid="{AB315AF7-6E61-41FF-B103-02B048860876}"/>
+    <hyperlink ref="C20" r:id="rId7" xr:uid="{E42397F9-DA6A-40BD-ACA8-EEB06E324F41}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId8"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
some analysis files added by kyo
</commit_message>
<xml_diff>
--- a/documents/payment.xlsx
+++ b/documents/payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\AbArts\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062C4BA3-8F0E-4B1D-A1A7-2ADFB6CDA74B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFCB8E-8FEB-4C80-94DB-6A72147582FF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fMRI task prep by kyo
</commit_message>
<xml_diff>
--- a/documents/payment.xlsx
+++ b/documents/payment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\AbArts\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFCB8E-8FEB-4C80-94DB-6A72147582FF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9B8BE3-F2E9-40B7-8AAD-6E280C3E3E96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="5040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>